<commit_message>
Persian feature description added
</commit_message>
<xml_diff>
--- a/DataSet/02_preprocessing_after_normalizing_values.xlsx
+++ b/DataSet/02_preprocessing_after_normalizing_values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="19545" windowHeight="8205"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="19545" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,10 +462,37 @@
   <dimension ref="A1:Z501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>